<commit_message>
Add initial experiment results of two stage approach
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -76,6 +76,15 @@
 - Evaluation auf fold_9</t>
   </si>
   <si>
+    <t xml:space="preserve">Gen-Modell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL-Modell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_beams=10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baseline (BART)</t>
   </si>
   <si>
@@ -83,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Classification (Binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_beams=20</t>
   </si>
 </sst>
 </file>
@@ -95,7 +107,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -123,11 +135,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,7 +221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,12 +282,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -306,7 +341,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -595,7 +630,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -726,40 +761,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="25.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
-      <c r="J1" s="5"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="15"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -767,9 +801,9 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -778,128 +812,227 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>56.0597</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2"/>
+      <c r="E7" s="0" t="n">
         <v>36.1088</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>51.3387</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="2"/>
+      <c r="I7" s="0" t="n">
         <v>51.2209</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="17"/>
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>55.8767</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2"/>
+      <c r="E9" s="0" t="n">
         <v>36.2574</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>51.9099</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="2"/>
+      <c r="I9" s="0" t="n">
         <v>51.7879</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="19" t="n">
         <v>57.3645</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="20"/>
+      <c r="E10" s="18" t="n">
         <v>37.3808</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="21"/>
+      <c r="G10" s="19" t="n">
         <v>52.7819</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="20"/>
+      <c r="I10" s="18" t="n">
         <v>52.7059</v>
       </c>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>56.0138</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="0" t="n">
+        <v>36.3498</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>51.5684</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="0" t="n">
+        <v>51.5018</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23"/>
+      <c r="B15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:I2"/>
+  <mergeCells count="9">
+    <mergeCell ref="C1:J2"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add initial validation results
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -10,7 +10,8 @@
   <sheets>
     <sheet name="splits_s777" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="splits_s17" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Beam_10" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="test_on_dev" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="st_val_data" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -72,7 +73,7 @@
     <t xml:space="preserve">Beschreibung</t>
   </si>
   <si>
-    <t xml:space="preserve">- Candidate generation parameters: num_beams=10, num_return_sequences=10
+    <t xml:space="preserve">- Candidate generation durch 10-fach CV → Predictions auf test sets bilden Input für das CL-Netzwerk
 - Evaluation auf fold_9</t>
   </si>
   <si>
@@ -107,7 +108,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -135,6 +136,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,15 +300,31 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,8 +336,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -341,7 +415,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -630,7 +704,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -764,10 +838,10 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="25.14"/>
   </cols>
@@ -884,122 +958,148 @@
       <c r="B7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="18" t="n">
         <v>56.0597</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="0" t="n">
+      <c r="D7" s="19"/>
+      <c r="E7" s="14" t="n">
         <v>36.1088</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="14"/>
+      <c r="G7" s="18" t="n">
         <v>51.3387</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="0" t="n">
+      <c r="H7" s="19"/>
+      <c r="I7" s="14" t="n">
         <v>51.2209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17"/>
       <c r="B9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="18" t="n">
         <v>55.8767</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="0" t="n">
+      <c r="D9" s="19"/>
+      <c r="E9" s="14" t="n">
         <v>36.2574</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="F9" s="14"/>
+      <c r="G9" s="18" t="n">
         <v>51.9099</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="0" t="n">
+      <c r="H9" s="19"/>
+      <c r="I9" s="14" t="n">
         <v>51.7879</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="19" t="n">
+      <c r="C10" s="21" t="n">
         <v>57.3645</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="18" t="n">
+      <c r="D10" s="22"/>
+      <c r="E10" s="23" t="n">
         <v>37.3808</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="19" t="n">
+      <c r="F10" s="24"/>
+      <c r="G10" s="21" t="n">
         <v>52.7819</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="18" t="n">
+      <c r="H10" s="22"/>
+      <c r="I10" s="23" t="n">
         <v>52.7059</v>
       </c>
-      <c r="J10" s="21"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="18" t="n">
         <v>56.0138</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="0" t="n">
+      <c r="D12" s="19"/>
+      <c r="E12" s="14" t="n">
         <v>36.3498</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="F12" s="14"/>
+      <c r="G12" s="18" t="n">
         <v>51.5684</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="0" t="n">
+      <c r="H12" s="19"/>
+      <c r="I12" s="14" t="n">
         <v>51.5018</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="27"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="27"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="28" t="n">
+        <v>57.3602</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="29" t="n">
+        <v>36.7845</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="28" t="n">
+        <v>53.239</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="29" t="n">
+        <v>53.208</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1"/>
@@ -1042,4 +1142,245 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="31" t="n">
+        <v>35.164</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33" t="n">
+        <v>17.5403</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="31" t="n">
+        <v>33.2457</v>
+      </c>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33" t="n">
+        <v>33.3624</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17"/>
+      <c r="B5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="34" t="n">
+        <v>33.7786</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="35" t="n">
+        <v>16.8929</v>
+      </c>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34" t="n">
+        <v>32.1405</v>
+      </c>
+      <c r="H5" s="32"/>
+      <c r="I5" s="35" t="n">
+        <v>32.4175</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17"/>
+      <c r="B6" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="37" t="n">
+        <v>34.7648</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39" t="n">
+        <v>18.0236</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="37" t="n">
+        <v>33.5192</v>
+      </c>
+      <c r="H6" s="38"/>
+      <c r="I6" s="39" t="n">
+        <v>33.7031</v>
+      </c>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="26"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>35.1119</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="29" t="n">
+        <v>17.4486</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="28" t="n">
+        <v>33.3119</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="29" t="n">
+        <v>33.4253</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="27"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="27"/>
+      <c r="B11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="28" t="n">
+        <v>35.419</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="29" t="n">
+        <v>16.7096</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="28" t="n">
+        <v>34.742</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="29" t="n">
+        <v>34.7925</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A8:A11"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add lower case support and add further initial validation set experiment results
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t xml:space="preserve">num_beams=20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DistilBert (binary, pretrained) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bert (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioReddit (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DistilRoberta (binary, pretrained)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioBERT (binary)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,6 +355,26 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,11 +399,11 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,7 +411,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,12 +419,20 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -415,7 +458,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -704,7 +747,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -838,10 +881,10 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="25.14"/>
   </cols>
@@ -1080,38 +1123,66 @@
       <c r="H14" s="19"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27"/>
-      <c r="B15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="28" t="n">
+      <c r="B15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="29" t="n">
         <v>57.3602</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="29" t="n">
+      <c r="D15" s="30"/>
+      <c r="E15" s="31" t="n">
         <v>36.7845</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="28" t="n">
+      <c r="F15" s="32"/>
+      <c r="G15" s="29" t="n">
         <v>53.239</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="29" t="n">
+      <c r="H15" s="30"/>
+      <c r="I15" s="31" t="n">
         <v>53.208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="33" t="n">
+        <v>53.8575</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="34" t="n">
+        <v>35.3438</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="33" t="n">
+        <v>49.7512</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="34" t="n">
+        <v>49.8102</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
+      <c r="B17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="33" t="n">
+        <v>56.0177</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="34" t="n">
+        <v>37.6264</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="33" t="n">
+        <v>51.9301</v>
+      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="34" t="n">
+        <v>51.9578</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1"/>
@@ -1149,16 +1220,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,75 +1288,75 @@
       <c r="A3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="31" t="n">
+      <c r="C3" s="36" t="n">
         <v>35.164</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33" t="n">
+      <c r="D3" s="37"/>
+      <c r="E3" s="38" t="n">
         <v>17.5403</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="31" t="n">
+      <c r="F3" s="38"/>
+      <c r="G3" s="36" t="n">
         <v>33.2457</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33" t="n">
+      <c r="H3" s="37"/>
+      <c r="I3" s="38" t="n">
         <v>33.3624</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17"/>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="34" t="n">
+      <c r="C5" s="39" t="n">
         <v>33.7786</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="35" t="n">
+      <c r="D5" s="37"/>
+      <c r="E5" s="40" t="n">
         <v>16.8929</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34" t="n">
+      <c r="F5" s="38"/>
+      <c r="G5" s="39" t="n">
         <v>32.1405</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="35" t="n">
+      <c r="H5" s="37"/>
+      <c r="I5" s="40" t="n">
         <v>32.4175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="37" t="n">
+      <c r="C6" s="42" t="n">
         <v>34.7648</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="39" t="n">
+      <c r="D6" s="43"/>
+      <c r="E6" s="44" t="n">
         <v>18.0236</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="37" t="n">
+      <c r="F6" s="45"/>
+      <c r="G6" s="42" t="n">
         <v>33.5192</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39" t="n">
+      <c r="H6" s="43"/>
+      <c r="I6" s="44" t="n">
         <v>33.7031</v>
       </c>
       <c r="J6" s="25"/>
@@ -1311,15 +1382,15 @@
         <v>35.1119</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="29" t="n">
+      <c r="E8" s="46" t="n">
         <v>17.4486</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="28" t="n">
+      <c r="G8" s="47" t="n">
         <v>33.3119</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="29" t="n">
+      <c r="I8" s="46" t="n">
         <v>33.4253</v>
       </c>
     </row>
@@ -1346,22 +1417,62 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27"/>
       <c r="B11" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C11" s="47" t="n">
         <v>35.419</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="29" t="n">
+      <c r="E11" s="46" t="n">
         <v>16.7096</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="28" t="n">
+      <c r="G11" s="47" t="n">
         <v>34.742</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="I11" s="29" t="n">
+      <c r="I11" s="46" t="n">
         <v>34.7925</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="18" t="n">
+        <v>34.8319</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="14" t="n">
+        <v>18.0046</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="18" t="n">
+        <v>33.5177</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="14" t="n">
+        <v>33.6209</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="18" t="n">
+        <v>33.4035</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="14" t="n">
+        <v>15.8741</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="18" t="n">
+        <v>31.6601</v>
+      </c>
+      <c r="H13" s="19"/>
+      <c r="I13" s="14" t="n">
+        <v>31.8336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set lower case as default for discriminator learning
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="splits_s777" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -46,25 +46,34 @@
     <t xml:space="preserve">std_dev</t>
   </si>
   <si>
+    <t xml:space="preserve">Baseline (BART)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HunFlair (1.030)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMLS (1.375)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard (1.157)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All (14.241)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline (25 Epochs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMLS(25 Epochs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pegasus-Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BART-Large</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HunFlair (1.030)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMLS (1.375)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hard (1.157)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All (14.241)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baseline (25 Epochs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMLS(25 Epochs)</t>
   </si>
   <si>
     <t xml:space="preserve">UMLS</t>
@@ -86,9 +95,6 @@
     <t xml:space="preserve">num_beams=10</t>
   </si>
   <si>
-    <t xml:space="preserve">Baseline (BART)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Classification (Sim – rougeL)</t>
   </si>
   <si>
@@ -98,19 +104,31 @@
     <t xml:space="preserve">num_beams=20</t>
   </si>
   <si>
-    <t xml:space="preserve">DistilBert (binary, pretrained) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bert (binary)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BioReddit (binary)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DistilRoberta (binary, pretrained)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BioBERT (binary)</t>
+    <t xml:space="preserve">&gt;&gt; DistilBert (binary, pretrained) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; Bert (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; BioReddit (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline (BART-LARGE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; Bert-cased (pretrained, binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baseline (PEGASUS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; DistilRoberta (binary, pretrained)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; BioBERT (binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; Bert-cased (binary, pretrained)</t>
   </si>
 </sst>
 </file>
@@ -242,7 +260,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,7 +393,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,14 +447,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -452,13 +466,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -717,6 +731,92 @@
       <c r="I11" s="12" t="n">
         <v>3.54904576894973</v>
       </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="n">
+        <v>53.39281</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>2.68914047548654</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>35.42576</v>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>3.07903050527272</v>
+      </c>
+      <c r="F13" s="9" t="n">
+        <v>50.18781</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <v>2.61641615590869</v>
+      </c>
+      <c r="H13" s="9" t="n">
+        <v>50.27211</v>
+      </c>
+      <c r="I13" s="10" t="n">
+        <v>2.62213875241186</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>53.98172</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>1.80861587563529</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <v>35.27203</v>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>2.22351279512847</v>
+      </c>
+      <c r="F14" s="9" t="n">
+        <v>50.55609</v>
+      </c>
+      <c r="G14" s="10" t="n">
+        <v>1.97602107147166</v>
+      </c>
+      <c r="H14" s="9" t="n">
+        <v>50.59783</v>
+      </c>
+      <c r="I14" s="13" t="n">
+        <v>2.05583847665618</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0"/>
+      <c r="D26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -747,7 +847,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -799,7 +899,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B3" s="14" t="n">
         <v>51.96418</v>
@@ -828,7 +928,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>50.61776</v>
@@ -878,23 +978,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -944,10 +1045,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -996,10 +1097,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C7" s="18" t="n">
         <v>56.0597</v>
@@ -1030,7 +1131,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17"/>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="18" t="n">
         <v>55.8767</v>
@@ -1051,7 +1152,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17"/>
       <c r="B10" s="20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" s="21" t="n">
         <v>57.3645</v>
@@ -1082,10 +1183,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C12" s="18" t="n">
         <v>56.0138</v>
@@ -1105,93 +1206,131 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="14"/>
+      <c r="B13" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="29" t="n">
+        <v>57.3602</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31" t="n">
+        <v>36.7845</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="29" t="n">
+        <v>53.239</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31" t="n">
+        <v>53.208</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="33" t="n">
+        <v>53.8575</v>
+      </c>
       <c r="D14" s="19"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="34" t="n">
+        <v>35.3438</v>
+      </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="33" t="n">
+        <v>49.7512</v>
+      </c>
       <c r="H14" s="19"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="29" t="n">
-        <v>57.3602</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31" t="n">
-        <v>36.7845</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="29" t="n">
-        <v>53.239</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31" t="n">
-        <v>53.208</v>
+      <c r="I14" s="34" t="n">
+        <v>49.8102</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="33" t="n">
+        <v>56.0177</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="34" t="n">
+        <v>37.6264</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="33" t="n">
+        <v>51.9301</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="34" t="n">
+        <v>51.9578</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="33" t="n">
-        <v>53.8575</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="34" t="n">
-        <v>35.3438</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="33" t="n">
-        <v>49.7512</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="34" t="n">
-        <v>49.8102</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="33" t="n">
-        <v>56.0177</v>
+        <v>29</v>
+      </c>
+      <c r="C17" s="18" t="n">
+        <v>54.2567</v>
       </c>
       <c r="D17" s="19"/>
-      <c r="E17" s="34" t="n">
-        <v>37.6264</v>
+      <c r="E17" s="14" t="n">
+        <v>35.3428</v>
       </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="33" t="n">
-        <v>51.9301</v>
+      <c r="G17" s="18" t="n">
+        <v>50.1313</v>
       </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="34" t="n">
-        <v>51.9578</v>
+      <c r="I17" s="14" t="n">
+        <v>49.8721</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="1"/>
+      <c r="B18" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="35" t="n">
+        <v>58.7029</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="35" t="n">
+        <v>40.0317</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="35" t="n">
+        <v>54.5167</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="35" t="n">
+        <v>54.471</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="14" t="n">
+        <v>56.3646</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="n">
+        <v>37.4169</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14" t="n">
+        <v>52.2305</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14" t="n">
+        <v>52.1585</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1203,7 +1342,7 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1220,24 +1359,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1286,77 +1425,77 @@
     </row>
     <row r="3" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="36" t="n">
+        <v>22</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="37" t="n">
         <v>35.164</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38" t="n">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39" t="n">
         <v>17.5403</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="36" t="n">
+      <c r="F3" s="39"/>
+      <c r="G3" s="37" t="n">
         <v>33.2457</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="38" t="n">
+      <c r="H3" s="38"/>
+      <c r="I3" s="39" t="n">
         <v>33.3624</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17"/>
-      <c r="B5" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="39" t="n">
+      <c r="B5" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="40" t="n">
         <v>33.7786</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="40" t="n">
+      <c r="D5" s="38"/>
+      <c r="E5" s="41" t="n">
         <v>16.8929</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39" t="n">
+      <c r="F5" s="39"/>
+      <c r="G5" s="40" t="n">
         <v>32.1405</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="40" t="n">
+      <c r="H5" s="38"/>
+      <c r="I5" s="41" t="n">
         <v>32.4175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17"/>
-      <c r="B6" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="42" t="n">
+      <c r="B6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="43" t="n">
         <v>34.7648</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44" t="n">
+      <c r="D6" s="44"/>
+      <c r="E6" s="45" t="n">
         <v>18.0236</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="42" t="n">
+      <c r="F6" s="46"/>
+      <c r="G6" s="43" t="n">
         <v>33.5192</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="44" t="n">
+      <c r="H6" s="44"/>
+      <c r="I6" s="45" t="n">
         <v>33.7031</v>
       </c>
       <c r="J6" s="25"/>
@@ -1373,24 +1512,24 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C8" s="18" t="n">
         <v>35.1119</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="46" t="n">
+      <c r="E8" s="34" t="n">
         <v>17.4486</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="47" t="n">
+      <c r="G8" s="33" t="n">
         <v>33.3119</v>
       </c>
       <c r="H8" s="19"/>
-      <c r="I8" s="46" t="n">
+      <c r="I8" s="34" t="n">
         <v>33.4253</v>
       </c>
     </row>
@@ -1406,33 +1545,43 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="33" t="n">
+        <v>35.419</v>
+      </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="34" t="n">
+        <v>16.7096</v>
+      </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="33" t="n">
+        <v>34.742</v>
+      </c>
       <c r="H10" s="19"/>
-      <c r="I10" s="14"/>
+      <c r="I10" s="34" t="n">
+        <v>34.7925</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27"/>
       <c r="B11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="47" t="n">
-        <v>35.419</v>
+        <v>33</v>
+      </c>
+      <c r="C11" s="18" t="n">
+        <v>34.8319</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="46" t="n">
-        <v>16.7096</v>
+      <c r="E11" s="14" t="n">
+        <v>18.0046</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="47" t="n">
-        <v>34.742</v>
+      <c r="G11" s="18" t="n">
+        <v>33.5177</v>
       </c>
       <c r="H11" s="19"/>
-      <c r="I11" s="46" t="n">
-        <v>34.7925</v>
+      <c r="I11" s="14" t="n">
+        <v>33.6209</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,40 +1589,116 @@
         <v>28</v>
       </c>
       <c r="C12" s="18" t="n">
-        <v>34.8319</v>
+        <v>33.4035</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="14" t="n">
-        <v>18.0046</v>
+        <v>15.8741</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="18" t="n">
-        <v>33.5177</v>
+        <v>31.6601</v>
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="14" t="n">
-        <v>33.6209</v>
+        <v>31.8336</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="18" t="n">
-        <v>33.4035</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="14" t="n">
-        <v>15.8741</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="18" t="n">
-        <v>31.6601</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="14" t="n">
-        <v>31.8336</v>
-      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>34.119</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="14" t="n">
+        <v>15.1702</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="18" t="n">
+        <v>31.5856</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="14" t="n">
+        <v>31.6906</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="18" t="n">
+        <v>33.702</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="14" t="n">
+        <v>15.8158</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="18" t="n">
+        <v>31.485</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="14" t="n">
+        <v>31.6527</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="18" t="n">
+        <v>33.6026</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="14" t="n">
+        <v>13.8294</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="18" t="n">
+        <v>31.02</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="14" t="n">
+        <v>30.9685</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1484,7 +1709,7 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Refactor prediction on validation set
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="splits_s777" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
   <si>
     <t xml:space="preserve">Modell</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">&gt;&gt; Bert-cased (pretrained, binary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; Bert-uncased (pretrained, binary) </t>
   </si>
   <si>
     <t xml:space="preserve">Baseline (PEGASUS)</t>
@@ -141,7 +144,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -169,11 +172,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,10 +396,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -472,7 +466,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -847,7 +841,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -980,11 +974,11 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.35"/>
@@ -1296,25 +1290,45 @@
       <c r="B18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="35" t="n">
+      <c r="C18" s="34" t="n">
         <v>58.7029</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="35" t="n">
+      <c r="E18" s="34" t="n">
         <v>40.0317</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="35" t="n">
+      <c r="G18" s="34" t="n">
         <v>54.5167</v>
       </c>
       <c r="H18" s="14"/>
-      <c r="I18" s="35" t="n">
+      <c r="I18" s="34" t="n">
         <v>54.471</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="14" t="n">
+        <v>58.7394</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="n">
+        <v>39.9298</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="n">
+        <v>54.2504</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14" t="n">
+        <v>54.3005</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21" s="14" t="n">
         <v>56.3646</v>
@@ -1359,13 +1373,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.92"/>
@@ -1427,75 +1441,75 @@
       <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="37" t="n">
+      <c r="C3" s="36" t="n">
         <v>35.164</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39" t="n">
+      <c r="D3" s="37"/>
+      <c r="E3" s="38" t="n">
         <v>17.5403</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="37" t="n">
+      <c r="F3" s="38"/>
+      <c r="G3" s="36" t="n">
         <v>33.2457</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39" t="n">
+      <c r="H3" s="37"/>
+      <c r="I3" s="38" t="n">
         <v>33.3624</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17"/>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="40" t="n">
+      <c r="C5" s="39" t="n">
         <v>33.7786</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="41" t="n">
+      <c r="D5" s="37"/>
+      <c r="E5" s="40" t="n">
         <v>16.8929</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="40" t="n">
+      <c r="F5" s="38"/>
+      <c r="G5" s="39" t="n">
         <v>32.1405</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="41" t="n">
+      <c r="H5" s="37"/>
+      <c r="I5" s="40" t="n">
         <v>32.4175</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17"/>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="43" t="n">
+      <c r="C6" s="42" t="n">
         <v>34.7648</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45" t="n">
+      <c r="D6" s="43"/>
+      <c r="E6" s="44" t="n">
         <v>18.0236</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="43" t="n">
+      <c r="F6" s="45"/>
+      <c r="G6" s="42" t="n">
         <v>33.5192</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45" t="n">
+      <c r="H6" s="43"/>
+      <c r="I6" s="44" t="n">
         <v>33.7031</v>
       </c>
       <c r="J6" s="25"/>
@@ -1546,7 +1560,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27"/>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="33" t="n">
         <v>35.419</v>
@@ -1566,7 +1580,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="18" t="n">
         <v>34.8319</v>
@@ -1638,7 +1652,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="18" t="n">
         <v>33.702</v>
@@ -1657,30 +1671,29 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
+      <c r="B17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>33.3759</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="G17" s="1"/>
+      <c r="E17" s="0" t="n">
+        <v>14.5256</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>30.5013</v>
+      </c>
       <c r="H17" s="2"/>
+      <c r="I17" s="0" t="n">
+        <v>30.7221</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="18" t="n">
-        <v>33.6026</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="14" t="n">
-        <v>13.8294</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="18" t="n">
-        <v>31.02</v>
-      </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="14" t="n">
-        <v>30.9685</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1"/>
@@ -1689,16 +1702,42 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="18" t="n">
+        <v>33.6026</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="14" t="n">
+        <v>13.8294</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="18" t="n">
+        <v>31.02</v>
+      </c>
+      <c r="H20" s="19"/>
+      <c r="I20" s="14" t="n">
+        <v>30.9685</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>